<commit_message>
29 Nov no. 1
</commit_message>
<xml_diff>
--- a/01.MODELO PERSEPOLIS/02.Ejecucion/04.Frente Comercial/Listado contactos CGLU/Contactos CGLU - Suministrados por la organización del evento.xlsx
+++ b/01.MODELO PERSEPOLIS/02.Ejecucion/04.Frente Comercial/Listado contactos CGLU/Contactos CGLU - Suministrados por la organización del evento.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johas\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28700" windowHeight="15680" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Contactos " sheetId="1" r:id="rId1"/>
@@ -12,11 +17,11 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -124,21 +129,12 @@
     <t>Marcos Daniel Pineda García</t>
   </si>
   <si>
-    <t>Isaías Chala Ibarguen</t>
-  </si>
-  <si>
     <t>Fabio David Velásquez Rivadeneira</t>
   </si>
   <si>
-    <t>Rodrigo armando Lara Sánchez</t>
-  </si>
-  <si>
     <t>Rafael Alejandro Martínez</t>
   </si>
   <si>
-    <t>César omar Rojas Ayala</t>
-  </si>
-  <si>
     <t>José Antonio Castro Meléndez</t>
   </si>
   <si>
@@ -149,9 +145,6 @@
   </si>
   <si>
     <t>Daniel Bernal Córdoba</t>
-  </si>
-  <si>
-    <t>Marcos Perez Jiménez</t>
   </si>
   <si>
     <t xml:space="preserve">josehuberaraujonieto@hotmail.com </t>
@@ -297,39 +290,12 @@
     <t>Arauca/Arauca</t>
   </si>
   <si>
-    <t>Atlantico/Barranquilla</t>
-  </si>
-  <si>
-    <t>Bolivar/Cartagena</t>
-  </si>
-  <si>
-    <t>Boyaca/Tunja</t>
-  </si>
-  <si>
-    <t>Caldas/Manizalez</t>
-  </si>
-  <si>
-    <t>Caqueta/Florencia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Casanare/Yopal </t>
   </si>
   <si>
-    <t xml:space="preserve">Cauca/Popayan </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cesar/Valledupar </t>
   </si>
   <si>
-    <t xml:space="preserve">Cordoba/Monteria </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Choco/Quibdo </t>
-  </si>
-  <si>
-    <t>Guania/Puerto Inirida</t>
-  </si>
-  <si>
     <t xml:space="preserve">Guajira/Riohacha </t>
   </si>
   <si>
@@ -351,27 +317,15 @@
     <t xml:space="preserve">Putumayo/Mocoa </t>
   </si>
   <si>
-    <t xml:space="preserve">Quindio/Armenia </t>
-  </si>
-  <si>
     <t xml:space="preserve">Risaralda/Pereira </t>
   </si>
   <si>
-    <t>San Andrés/Alcaldía Municipal Providencia y Santa Cantalina Islas</t>
-  </si>
-  <si>
     <t>Sucre/Sincelejo</t>
   </si>
   <si>
     <t xml:space="preserve">Tolima/Ibagué </t>
   </si>
   <si>
-    <t>Valle del cauca/Santiago de cali</t>
-  </si>
-  <si>
-    <t>Vaupes/Mitù</t>
-  </si>
-  <si>
     <t>Vichada/Puerto Carreño</t>
   </si>
   <si>
@@ -558,29 +512,80 @@
     <t>César Cristian Gómez Castro</t>
   </si>
   <si>
-    <t>Efraín Rivera Roldan</t>
-  </si>
-  <si>
     <t>Guillermo Alfonso Jaramillo Martínez</t>
   </si>
   <si>
-    <t>José huber Araujo Nieto</t>
-  </si>
-  <si>
-    <t>Juan pablo Gallo Maya</t>
-  </si>
-  <si>
     <t>Wilmar Orlando Barbosa Rozo</t>
   </si>
   <si>
     <t>tratamiento</t>
+  </si>
+  <si>
+    <t>Rodrigo Armando Lara Sánchez</t>
+  </si>
+  <si>
+    <t>Caquetá/Florencia</t>
+  </si>
+  <si>
+    <t>San Andrés/Alcaldía Municipal Providencia y Santa Catalina Islas</t>
+  </si>
+  <si>
+    <t>Guanía/Puerto Inírida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quindío/Armenia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cauca/Popayán </t>
+  </si>
+  <si>
+    <t>César Omar Rojas Ayala</t>
+  </si>
+  <si>
+    <t>Vaupés/Mitú</t>
+  </si>
+  <si>
+    <t>Isaías Chala Ibargüen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choco/Quibdó </t>
+  </si>
+  <si>
+    <t>José Huber Araujo Nieto</t>
+  </si>
+  <si>
+    <t>Caldas/Manizales</t>
+  </si>
+  <si>
+    <t>Bolívar/Cartagena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Córdoba/Montería </t>
+  </si>
+  <si>
+    <t>Marcos Pérez Jiménez</t>
+  </si>
+  <si>
+    <t>Valle del cauca/Santiago de Cali</t>
+  </si>
+  <si>
+    <t>Boyacá/Tunja</t>
+  </si>
+  <si>
+    <t>Atlántico/Barranquilla</t>
+  </si>
+  <si>
+    <t>Juan Pablo Gallo Maya</t>
+  </si>
+  <si>
+    <t>Efraín Rivera Roldán</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1107,7 +1112,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1117,39 +1122,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" outlineLevelCol="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="13.5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="37" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="45" style="2" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="31.83203125" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="17.33203125" style="3" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="31.85546875" style="2" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="17.28515625" style="3" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="31" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="69" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="37.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="22.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="52">
+    <row r="1" spans="1:12" ht="54">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>1</v>
@@ -1161,7 +1166,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>3</v>
@@ -1175,62 +1180,62 @@
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="7" customFormat="1">
       <c r="A3" s="9" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>88</v>
+        <v>158</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1">
@@ -1238,10 +1243,10 @@
         <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="1" t="s">
@@ -1251,114 +1256,114 @@
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="7" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="7" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>104</v>
+        <v>159</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="7" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="7" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>20</v>
@@ -1371,84 +1376,84 @@
         <v>9</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="7" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="7" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>163</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="7" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>25</v>
@@ -1461,84 +1466,84 @@
         <v>9</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="7" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="7" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="7" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>23</v>
@@ -1549,76 +1554,76 @@
         <v>9</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="7" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="7" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="7" customFormat="1">
@@ -1626,10 +1631,10 @@
         <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="1" t="s">
@@ -1639,76 +1644,76 @@
         <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="7" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="7" customFormat="1">
       <c r="A19" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="7" customFormat="1">
@@ -1716,59 +1721,59 @@
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="7" customFormat="1">
       <c r="A21" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="7" customFormat="1">
@@ -1776,29 +1781,29 @@
         <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>85</v>
+        <v>169</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="7" customFormat="1">
@@ -1806,89 +1811,89 @@
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:12" s="7" customFormat="1">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="7" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="7" customFormat="1">
@@ -1896,119 +1901,119 @@
         <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="7" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="7" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>157</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="7" customFormat="1">
       <c r="A29" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2056,32 +2061,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.1640625" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39">
+    <row r="1" spans="1:12" ht="54">
       <c r="A1" s="11" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>1</v>
@@ -2093,7 +2098,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>3</v>
@@ -2110,31 +2115,31 @@
         <v>144</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="17">
         <v>3103008080</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K2" s="18"/>
       <c r="L2" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2142,31 +2147,31 @@
         <v>143</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="17">
         <v>4462397</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="14"/>
       <c r="J3" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K3" s="18"/>
       <c r="L3" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2174,29 +2179,29 @@
         <v>153</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="17">
         <v>3114457302</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
       <c r="J4" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K4" s="18"/>
       <c r="L4" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2204,29 +2209,29 @@
         <v>163</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="17">
         <v>3115395807</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
       <c r="J5" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K5" s="18"/>
       <c r="L5" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2234,13 +2239,13 @@
         <v>155</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="17">
@@ -2250,11 +2255,11 @@
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
       <c r="J6" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2262,29 +2267,29 @@
         <v>159</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="17">
         <v>3123770396</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2292,31 +2297,31 @@
         <v>154</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="17">
         <v>3143347049</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K8" s="18"/>
       <c r="L8" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -2324,29 +2329,29 @@
         <v>157</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="17">
         <v>3158445075</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
       <c r="J9" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K9" s="18"/>
       <c r="L9" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -2354,29 +2359,29 @@
         <v>151</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="17">
         <v>3167441051</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -2384,29 +2389,29 @@
         <v>148</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="17">
         <v>3007476712</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -2414,29 +2419,29 @@
         <v>165</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="17">
         <v>3112527189</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
       <c r="J12" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -2444,10 +2449,10 @@
         <v>167</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>8</v>
@@ -2457,16 +2462,16 @@
         <v>3105632535</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2474,29 +2479,29 @@
         <v>156</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="17">
         <v>3006006910</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -2504,29 +2509,29 @@
         <v>147</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="17">
         <v>3133239496</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -2534,29 +2539,29 @@
         <v>158</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="17">
         <v>3132308360</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="14" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>